<commit_message>
PCB and BOM update
</commit_message>
<xml_diff>
--- a/- PCB -/SUMEC SMD-V2/bom/Complete BOM.xlsx
+++ b/- PCB -/SUMEC SMD-V2/bom/Complete BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\GitHub\RoboCop\- PCB -\SUMEC SMD-V2\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A9F268-ED57-4DA1-A3CE-38412A4CC644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D40B48-E98B-4868-A49E-9F89D7FFE1A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="133">
   <si>
     <t>Id</t>
   </si>
@@ -47,18 +47,12 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>IC2,IC3</t>
-  </si>
-  <si>
     <t>DRV8874</t>
   </si>
   <si>
     <t>DRV8874PWPR</t>
   </si>
   <si>
-    <t>SW1,SW3,SW2</t>
-  </si>
-  <si>
     <t>SW_SPST_B3U-1000P</t>
   </si>
   <si>
@@ -98,9 +92,6 @@
     <t>R_0805_2012Metric_Pad1.20x1.40mm_HandSolder</t>
   </si>
   <si>
-    <t>J5</t>
-  </si>
-  <si>
     <t>USB_Type_C</t>
   </si>
   <si>
@@ -131,24 +122,12 @@
     <t>100nF</t>
   </si>
   <si>
-    <t>J7,J6,J8</t>
-  </si>
-  <si>
     <t>Molex_PicoBlade_53398-0671_1x06-1MP_P1.25mm_Vertical</t>
   </si>
   <si>
     <t>Conn_01x06_Pin</t>
   </si>
   <si>
-    <t>IC1</t>
-  </si>
-  <si>
-    <t>XT30U-M_1x02_P5.0mm_Vertical</t>
-  </si>
-  <si>
-    <t>XT30U-F</t>
-  </si>
-  <si>
     <t>U3</t>
   </si>
   <si>
@@ -173,27 +152,18 @@
     <t>TSOP382xx</t>
   </si>
   <si>
-    <t>SW4</t>
-  </si>
-  <si>
     <t>Custom_SPDT_4.8mm_Switch</t>
   </si>
   <si>
     <t>SW_DPDT_x2</t>
   </si>
   <si>
-    <t>J4,J10,J9</t>
-  </si>
-  <si>
     <t>Molex_PicoBlade_53398-0371_1x03-1MP_P1.25mm_Vertical</t>
   </si>
   <si>
     <t>Conn_01x03_Pin</t>
   </si>
   <si>
-    <t>R4</t>
-  </si>
-  <si>
     <t>0R</t>
   </si>
   <si>
@@ -218,27 +188,12 @@
     <t>Link</t>
   </si>
   <si>
-    <t>R1,R2</t>
-  </si>
-  <si>
-    <t>R5,R6</t>
-  </si>
-  <si>
-    <t>C1,C18</t>
-  </si>
-  <si>
     <t>220R</t>
   </si>
   <si>
-    <t>D1,D2</t>
-  </si>
-  <si>
     <t>10uF</t>
   </si>
   <si>
-    <t>22nF</t>
-  </si>
-  <si>
     <t>Molex_PicoBlade_53261-0471_1x04-1MP_P1.25mm_Horizontal</t>
   </si>
   <si>
@@ -251,9 +206,6 @@
     <t>QRE1113</t>
   </si>
   <si>
-    <t>H1,H3,H2 - H1,H2</t>
-  </si>
-  <si>
     <t>R10 - R3,R1</t>
   </si>
   <si>
@@ -266,18 +218,9 @@
     <t>Reserve</t>
   </si>
   <si>
-    <t>R3,R8</t>
-  </si>
-  <si>
-    <t>Logo, R2D2</t>
-  </si>
-  <si>
     <t>C3,C5,C10,C11,C12,C13,C14,C15,C16</t>
   </si>
   <si>
-    <t>Diode_SMD:D_1206_3216Metric_Pad1.42x1.75mm_HandSolder</t>
-  </si>
-  <si>
     <t>R_1206_3216Metric_Pad1.30x1.75mm_HandSolder</t>
   </si>
   <si>
@@ -363,6 +306,132 @@
   </si>
   <si>
     <t>C2,C4,C6,C7,C8,C9,C17,C19</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>100nF.boot</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>10uF.shrp</t>
+  </si>
+  <si>
+    <t>C15,C14</t>
+  </si>
+  <si>
+    <t>10k.mcu</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>100nF.en</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>100nF.mcu</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>J10,J8,J7</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>SW2</t>
+  </si>
+  <si>
+    <t>Logo</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>XT30PW-M</t>
+  </si>
+  <si>
+    <t>AMASS_XT30PW-M</t>
+  </si>
+  <si>
+    <t>J11</t>
+  </si>
+  <si>
+    <t>J5,J4,J6</t>
+  </si>
+  <si>
+    <t>C13,C5,C6</t>
+  </si>
+  <si>
+    <t>D2,D1</t>
+  </si>
+  <si>
+    <t>R7,R6</t>
+  </si>
+  <si>
+    <t>D_1206_3216Metric_Pad1.42x1.75mm_HandSolder</t>
+  </si>
+  <si>
+    <t>10uF.hb</t>
+  </si>
+  <si>
+    <t>C9,C10</t>
+  </si>
+  <si>
+    <t>R2,R1</t>
+  </si>
+  <si>
+    <t>10uF.stabl</t>
+  </si>
+  <si>
+    <t>C19,C17,C18,C16</t>
+  </si>
+  <si>
+    <t>100nF.hb</t>
+  </si>
+  <si>
+    <t>C7,C8</t>
+  </si>
+  <si>
+    <t>22nF.hb</t>
+  </si>
+  <si>
+    <t>C3,C4</t>
+  </si>
+  <si>
+    <t>R2D2</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>SW1,SW4,SW3</t>
+  </si>
+  <si>
+    <t>IC1,IC2</t>
+  </si>
+  <si>
+    <t>Designation</t>
+  </si>
+  <si>
+    <t>H1,H3,H2 - H1, H2</t>
   </si>
 </sst>
 </file>
@@ -1384,18 +1453,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="B34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51:F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="35.81640625" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" customWidth="1"/>
+    <col min="3" max="3" width="19.6328125" customWidth="1"/>
     <col min="4" max="4" width="57.08984375" customWidth="1"/>
-    <col min="5" max="5" width="25.453125" customWidth="1"/>
+    <col min="5" max="5" width="55" customWidth="1"/>
     <col min="6" max="6" width="35.6328125" customWidth="1"/>
     <col min="7" max="7" width="23.90625" customWidth="1"/>
     <col min="8" max="8" width="7.26953125" customWidth="1"/>
@@ -1417,13 +1486,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="F1" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>60</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>76</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>3</v>
@@ -1434,19 +1503,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="C2" s="1">
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="H2" s="1">
         <v>2</v>
@@ -1457,19 +1526,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="H3" s="1">
         <v>1</v>
@@ -1480,19 +1549,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>62</v>
+        <v>116</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="H4" s="1">
         <v>2</v>
@@ -1503,19 +1572,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="H5" s="1">
         <v>4</v>
@@ -1526,19 +1595,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C6" s="1">
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="H6" s="1">
         <v>3</v>
@@ -1549,16 +1618,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>77</v>
+        <v>128</v>
       </c>
       <c r="C7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>78</v>
+        <v>127</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="13"/>
@@ -1571,19 +1640,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>63</v>
+        <v>126</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="H8" s="1">
         <v>2</v>
@@ -1594,19 +1663,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="C9" s="1">
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="H9" s="1">
         <v>8</v>
@@ -1617,19 +1686,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="C10" s="1">
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="H10" s="1">
         <v>9</v>
@@ -1640,19 +1709,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="H11" s="1">
         <v>2</v>
@@ -1663,19 +1732,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>80</v>
+        <v>117</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="H12" s="1">
         <v>1</v>
@@ -1686,16 +1755,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="13"/>
@@ -1708,16 +1777,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="13"/>
@@ -1730,19 +1799,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="H15" s="1">
         <v>1</v>
@@ -1753,19 +1822,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>49</v>
+        <v>105</v>
       </c>
       <c r="C16" s="1">
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="H16" s="1">
         <v>3</v>
@@ -1776,19 +1845,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="H17" s="1">
         <v>1</v>
@@ -1799,19 +1868,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>113</v>
       </c>
       <c r="C18" s="1">
         <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="H18" s="1">
         <v>3</v>
@@ -1822,19 +1891,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="H19" s="1">
         <v>1</v>
@@ -1845,19 +1914,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="H20" s="1">
         <v>1</v>
@@ -1868,19 +1937,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="F21" s="14" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="H21" s="1">
         <v>1</v>
@@ -1891,19 +1960,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="H22" s="1">
         <v>1</v>
@@ -1914,19 +1983,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="H23" s="1">
         <v>1</v>
@@ -1937,19 +2006,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="H24" s="1">
         <v>1</v>
@@ -1960,19 +2029,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>35</v>
+        <v>112</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>37</v>
+        <v>110</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="H25" s="1">
         <v>1</v>
@@ -1983,19 +2052,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>4</v>
+        <v>130</v>
       </c>
       <c r="C26" s="1">
         <v>2</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="F26" s="14" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="H26" s="1">
         <v>2</v>
@@ -2006,19 +2075,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>7</v>
+        <v>129</v>
       </c>
       <c r="C27" s="1">
         <v>3</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="H27" s="1">
         <v>3</v>
@@ -2029,19 +2098,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="C28" s="1">
         <v>1</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="H28" s="1">
         <v>1</v>
@@ -2052,16 +2121,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>72</v>
+        <v>132</v>
       </c>
       <c r="C29" s="1">
         <v>5</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="13"/>
@@ -2074,19 +2143,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C30" s="1">
         <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="H30" s="1">
         <v>3</v>
@@ -2104,7 +2173,7 @@
       <c r="B33" s="1"/>
       <c r="C33">
         <f>SUM(C2:C32)</f>
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -2119,50 +2188,367 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="3"/>
+      <c r="B35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="3"/>
+      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
-      <c r="F37" s="4"/>
+      <c r="B37" s="1">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
+      <c r="B38" s="1">
+        <v>3</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B39" s="1">
+        <v>4</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" s="1">
+        <v>3</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B40" s="1">
+        <v>5</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D40" s="1">
+        <v>2</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
+      <c r="B41" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
+      <c r="B42" s="1">
+        <v>7</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D42" s="1">
+        <v>2</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
+      <c r="B43" s="1">
+        <v>8</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
+      <c r="B44" s="1">
+        <v>9</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D44" s="1">
+        <v>4</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B45" s="1">
+        <v>10</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D45" s="1">
+        <v>2</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B46" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B47" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B48" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B49" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B50" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B51" s="1">
+        <v>16</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F51" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B52" s="1">
+        <v>17</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D52" s="1">
+        <v>1</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B53" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B54" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B55" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B56" s="1">
+        <v>21</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D56" s="1">
+        <v>1</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B57" s="1">
+        <v>22</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D57" s="1">
+        <v>1</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B58" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B59" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B60" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B61" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B62" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B63" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B64" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B65" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B66" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B67" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B68" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B69" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B70" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B71" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
BOM update, cast iam
</commit_message>
<xml_diff>
--- a/- PCB -/SUMEC SMD-V2/bom/Complete BOM.xlsx
+++ b/- PCB -/SUMEC SMD-V2/bom/Complete BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\GitHub\RoboCop\- PCB -\SUMEC SMD-V2\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9B437B-95F0-4A93-A1F5-33A296B88127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112C58A9-DAB3-488A-8BFE-82975BA1C0E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="120">
   <si>
     <t>Id</t>
   </si>
@@ -383,17 +383,23 @@
     <t>CONNECTOR 1x3</t>
   </si>
   <si>
-    <t>15 + 4 pujceno</t>
-  </si>
-  <si>
     <t>Green-Yellow LED, 20mA, 1.9V, mouser</t>
+  </si>
+  <si>
+    <t>100?</t>
+  </si>
+  <si>
+    <t>50?</t>
+  </si>
+  <si>
+    <t>15 + 4 pujceno + 10 doma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -579,6 +585,13 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="41">
     <fill>
@@ -985,7 +998,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1039,6 +1052,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1419,8 +1435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="77" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1481,7 +1497,9 @@
       <c r="F2" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1">
+        <v>20</v>
+      </c>
       <c r="H2" s="1">
         <v>1</v>
       </c>
@@ -1532,7 +1550,9 @@
       <c r="F4" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1">
+        <v>20</v>
+      </c>
       <c r="H4" s="1">
         <v>2</v>
       </c>
@@ -1556,7 +1576,9 @@
       <c r="F5" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1">
+        <v>20</v>
+      </c>
       <c r="H5" s="1">
         <v>4</v>
       </c>
@@ -1580,7 +1602,9 @@
       <c r="F6" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6" s="1">
+        <v>20</v>
+      </c>
       <c r="H6" s="1">
         <v>5</v>
       </c>
@@ -1626,7 +1650,9 @@
       <c r="F8" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1">
+        <v>20</v>
+      </c>
       <c r="H8" s="1">
         <v>2</v>
       </c>
@@ -1651,7 +1677,9 @@
       <c r="F9" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="H9" s="1">
         <v>8</v>
       </c>
@@ -1675,7 +1703,9 @@
       <c r="F10" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="H10" s="1">
         <v>9</v>
       </c>
@@ -1699,7 +1729,9 @@
       <c r="F11" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="G11" s="13"/>
+      <c r="G11" s="21">
+        <v>10</v>
+      </c>
       <c r="H11" s="1">
         <v>1</v>
       </c>
@@ -1725,7 +1757,9 @@
       <c r="F12" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1">
+        <v>10</v>
+      </c>
       <c r="H12" s="1">
         <v>1</v>
       </c>
@@ -1747,9 +1781,11 @@
         <v>25</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="G13" s="1"/>
+        <v>116</v>
+      </c>
+      <c r="G13" s="1">
+        <v>20</v>
+      </c>
       <c r="H13" s="1">
         <v>1</v>
       </c>
@@ -1843,7 +1879,9 @@
       <c r="F17" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="G17" s="1"/>
+      <c r="G17" s="1">
+        <v>4</v>
+      </c>
       <c r="H17" s="1">
         <v>1</v>
       </c>
@@ -1867,7 +1905,9 @@
       <c r="F18" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="G18" s="1"/>
+      <c r="G18" s="1">
+        <v>4</v>
+      </c>
       <c r="H18" s="1">
         <v>3</v>
       </c>
@@ -1891,7 +1931,9 @@
       <c r="F19" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="G19" s="1"/>
+      <c r="G19" s="1">
+        <v>4</v>
+      </c>
       <c r="H19" s="1">
         <v>1</v>
       </c>
@@ -1915,7 +1957,9 @@
       <c r="F20" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="G20" s="1"/>
+      <c r="G20" s="1">
+        <v>7</v>
+      </c>
       <c r="H20" s="1">
         <v>3</v>
       </c>
@@ -1939,7 +1983,9 @@
       <c r="F21" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="G21" s="1"/>
+      <c r="G21" s="1">
+        <v>6</v>
+      </c>
       <c r="H21" s="1">
         <v>1</v>
       </c>
@@ -1963,7 +2009,9 @@
       <c r="F22" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="G22" s="20"/>
+      <c r="G22" s="20">
+        <v>3</v>
+      </c>
       <c r="H22" s="1">
         <v>1</v>
       </c>
@@ -1987,7 +2035,9 @@
       <c r="F23" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="G23" s="20"/>
+      <c r="G23" s="20">
+        <v>3</v>
+      </c>
       <c r="H23" s="1">
         <v>1</v>
       </c>
@@ -2037,7 +2087,9 @@
       <c r="F25" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="G25" s="1"/>
+      <c r="G25" s="1">
+        <v>3</v>
+      </c>
       <c r="H25" s="1">
         <v>1</v>
       </c>
@@ -2111,7 +2163,9 @@
       <c r="F28" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="G28" s="1"/>
+      <c r="G28" s="1">
+        <v>5</v>
+      </c>
       <c r="H28" s="1">
         <v>2</v>
       </c>
@@ -2136,7 +2190,7 @@
         <v>63</v>
       </c>
       <c r="G29" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H29" s="1">
         <v>3</v>
@@ -2208,7 +2262,7 @@
         <v>60</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="H32" s="1">
         <v>3</v>
@@ -2451,5 +2505,6 @@
     <hyperlink ref="F33" r:id="rId28" xr:uid="{6ABF2726-A5C3-4787-BAF7-20B3D754FCE4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>